<commit_message>
Fixing themes for Telstra Histogram file
</commit_message>
<xml_diff>
--- a/result_for_histogram/Facebook/telstra_fb_post_hist.xlsx
+++ b/result_for_histogram/Facebook/telstra_fb_post_hist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magic\Desktop\Bus-Analytics Study Materials\Semester 2_2023\ETC5543 - Business Analytics Creative Activity\Forethought\Main Project\GitHub\Pre-Analysis\nlp_result_data\result_for_histogram\Facebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201EDF61-33BD-4680-BEE0-914197847B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662F8FE8-F60B-48BE-8603-35E24C63AA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,22 +35,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Theme1</t>
-  </si>
-  <si>
-    <t>Theme2</t>
-  </si>
-  <si>
-    <t>Theme3</t>
-  </si>
-  <si>
-    <t>Theme4</t>
-  </si>
-  <si>
     <t>Themes</t>
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Theme_1:Technical_Issues_and_Resolutions</t>
+  </si>
+  <si>
+    <t>Theme_2:Product_and_Service_Updates</t>
+  </si>
+  <si>
+    <t>Theme_3:Data_Breach_and_Privacy_Concerns</t>
+  </si>
+  <si>
+    <t>Theme_4:Customer_Support_and_Assistance</t>
   </si>
 </sst>
 </file>
@@ -407,26 +407,27 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="6" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>21</v>
@@ -434,7 +435,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>25</v>
@@ -442,7 +443,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -450,7 +451,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>18</v>

</xml_diff>